<commit_message>
updated logging to new folders,
</commit_message>
<xml_diff>
--- a/autoast/auto_ast_v3_Breville_folium_maps/gr_2025_26_jobs.xlsx
+++ b/autoast/auto_ast_v3_Breville_folium_maps/gr_2025_26_jobs.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,12 +29,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
       <sz val="11"/>
     </font>
     <font>
@@ -144,9 +138,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -180,7 +171,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -189,10 +180,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -599,155 +593,155 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="23.57642857142857" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
-    <col width="145.7192857142857" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
+    <col width="23.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="145.7192857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
     <col width="17.71928571428571" bestFit="1" customWidth="1" style="20" min="3" max="3"/>
     <col width="23.14785714285714" bestFit="1" customWidth="1" style="20" min="4" max="4"/>
     <col width="39.43357142857143" bestFit="1" customWidth="1" style="20" min="5" max="5"/>
-    <col width="171.7192857142857" bestFit="1" customWidth="1" style="6" min="6" max="6"/>
+    <col width="171.7192857142857" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
     <col width="34.005" bestFit="1" customWidth="1" style="21" min="7" max="7"/>
     <col width="26.86214285714286" bestFit="1" customWidth="1" style="21" min="8" max="8"/>
     <col width="29.005" bestFit="1" customWidth="1" style="21" min="9" max="9"/>
     <col width="21.005" bestFit="1" customWidth="1" style="21" min="10" max="10"/>
     <col width="21.29071428571428" bestFit="1" customWidth="1" style="21" min="11" max="11"/>
     <col width="13.71928571428571" bestFit="1" customWidth="1" style="21" min="12" max="12"/>
-    <col width="14.71928571428571" bestFit="1" customWidth="1" style="6" min="13" max="13"/>
+    <col width="14.71928571428571" bestFit="1" customWidth="1" style="5" min="13" max="13"/>
     <col width="11.57642857142857" bestFit="1" customWidth="1" style="20" min="14" max="14"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>region</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>feature_layer</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>crown_file_number</t>
         </is>
       </c>
-      <c r="D1" s="10" t="inlineStr">
+      <c r="D1" s="9" t="inlineStr">
         <is>
           <t>disposition_number</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>parcel_number</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" s="8" t="inlineStr">
         <is>
           <t>output_directory</t>
         </is>
       </c>
-      <c r="G1" s="12" t="inlineStr">
+      <c r="G1" s="11" t="inlineStr">
         <is>
           <t>output_directory_same_as_input</t>
         </is>
       </c>
-      <c r="H1" s="12" t="inlineStr">
+      <c r="H1" s="11" t="inlineStr">
         <is>
           <t>dont_overwrite_outputs</t>
         </is>
       </c>
-      <c r="I1" s="12" t="inlineStr">
+      <c r="I1" s="11" t="inlineStr">
         <is>
           <t>skip_conflicts_and_constraints</t>
         </is>
       </c>
-      <c r="J1" s="12" t="inlineStr">
+      <c r="J1" s="11" t="inlineStr">
         <is>
           <t>suppress_map_creation</t>
         </is>
       </c>
-      <c r="K1" s="12" t="inlineStr">
+      <c r="K1" s="11" t="inlineStr">
         <is>
           <t>add_maps_to_current</t>
         </is>
       </c>
-      <c r="L1" s="12" t="inlineStr">
+      <c r="L1" s="11" t="inlineStr">
         <is>
           <t>run_as_fcbc</t>
         </is>
       </c>
-      <c r="M1" s="9" t="inlineStr">
+      <c r="M1" s="8" t="inlineStr">
         <is>
           <t>ast_condition</t>
         </is>
       </c>
-      <c r="N1" s="11" t="inlineStr">
+      <c r="N1" s="10" t="inlineStr">
         <is>
           <t>file_number</t>
         </is>
       </c>
-      <c r="O1" s="13" t="n"/>
+      <c r="O1" s="12" t="n"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="14" t="inlineStr">
+      <c r="A2" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
       </c>
-      <c r="B2" s="15" t="inlineStr">
+      <c r="B2" s="14" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\632\632.shp</t>
         </is>
       </c>
-      <c r="C2" s="16" t="n"/>
-      <c r="D2" s="16" t="n"/>
-      <c r="E2" s="16" t="n"/>
-      <c r="F2" s="15" t="inlineStr">
+      <c r="C2" s="15" t="n"/>
+      <c r="D2" s="15" t="n"/>
+      <c r="E2" s="15" t="n"/>
+      <c r="F2" s="14" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\1</t>
         </is>
       </c>
-      <c r="G2" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H2" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I2" s="17" t="inlineStr">
+      <c r="G2" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H2" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I2" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="J2" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K2" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L2" s="17" t="inlineStr">
+      <c r="J2" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K2" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L2" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M2" s="14" t="inlineStr">
+      <c r="M2" s="17" t="inlineStr">
         <is>
           <t>COMPLETE</t>
         </is>
       </c>
       <c r="N2" s="18" t="n"/>
-      <c r="O2" s="13" t="n"/>
+      <c r="O2" s="12" t="n"/>
     </row>
     <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="14" t="inlineStr">
+      <c r="A3" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -757,54 +751,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\634\634.shp</t>
         </is>
       </c>
-      <c r="C3" s="16" t="n"/>
-      <c r="D3" s="16" t="n"/>
-      <c r="E3" s="16" t="n"/>
-      <c r="F3" s="15" t="inlineStr">
+      <c r="C3" s="15" t="n"/>
+      <c r="D3" s="15" t="n"/>
+      <c r="E3" s="15" t="n"/>
+      <c r="F3" s="14" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\2</t>
         </is>
       </c>
-      <c r="G3" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H3" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I3" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J3" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K3" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L3" s="17" t="inlineStr">
+      <c r="G3" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H3" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I3" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J3" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K3" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L3" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M3" s="14" t="inlineStr">
+      <c r="M3" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
       <c r="N3" s="18" t="n"/>
-      <c r="O3" s="4" t="n"/>
+      <c r="O3" s="3" t="n"/>
     </row>
     <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="14" t="inlineStr">
+      <c r="A4" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -814,54 +808,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\635\635.shp</t>
         </is>
       </c>
-      <c r="C4" s="16" t="n"/>
-      <c r="D4" s="16" t="n"/>
-      <c r="E4" s="16" t="n"/>
-      <c r="F4" s="15" t="inlineStr">
+      <c r="C4" s="15" t="n"/>
+      <c r="D4" s="15" t="n"/>
+      <c r="E4" s="15" t="n"/>
+      <c r="F4" s="14" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\3</t>
         </is>
       </c>
-      <c r="G4" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H4" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I4" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J4" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K4" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L4" s="17" t="inlineStr">
+      <c r="G4" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H4" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I4" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J4" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K4" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L4" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M4" s="14" t="inlineStr">
+      <c r="M4" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N4" s="16" t="n"/>
-      <c r="O4" s="7" t="n"/>
+      <c r="N4" s="15" t="n"/>
+      <c r="O4" s="6" t="n"/>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="14" t="inlineStr">
+      <c r="A5" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -871,54 +865,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\636\636.shp</t>
         </is>
       </c>
-      <c r="C5" s="16" t="n"/>
-      <c r="D5" s="16" t="n"/>
-      <c r="E5" s="16" t="n"/>
-      <c r="F5" s="15" t="inlineStr">
+      <c r="C5" s="15" t="n"/>
+      <c r="D5" s="15" t="n"/>
+      <c r="E5" s="15" t="n"/>
+      <c r="F5" s="14" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\4</t>
         </is>
       </c>
-      <c r="G5" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H5" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I5" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J5" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K5" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L5" s="17" t="inlineStr">
+      <c r="G5" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H5" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I5" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J5" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K5" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L5" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M5" s="14" t="inlineStr">
+      <c r="M5" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N5" s="16" t="n"/>
-      <c r="O5" s="7" t="n"/>
+      <c r="N5" s="15" t="n"/>
+      <c r="O5" s="6" t="n"/>
     </row>
     <row r="6" ht="19.5" customHeight="1">
-      <c r="A6" s="14" t="inlineStr">
+      <c r="A6" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -928,54 +922,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\637\637.shp</t>
         </is>
       </c>
-      <c r="C6" s="16" t="n"/>
-      <c r="D6" s="16" t="n"/>
-      <c r="E6" s="16" t="n"/>
-      <c r="F6" s="15" t="inlineStr">
+      <c r="C6" s="15" t="n"/>
+      <c r="D6" s="15" t="n"/>
+      <c r="E6" s="15" t="n"/>
+      <c r="F6" s="14" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\5</t>
         </is>
       </c>
-      <c r="G6" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H6" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I6" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J6" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K6" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L6" s="17" t="inlineStr">
+      <c r="G6" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H6" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I6" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J6" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K6" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L6" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M6" s="14" t="inlineStr">
+      <c r="M6" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N6" s="16" t="n"/>
-      <c r="O6" s="7" t="n"/>
+      <c r="N6" s="15" t="n"/>
+      <c r="O6" s="6" t="n"/>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="14" t="inlineStr">
+      <c r="A7" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -985,54 +979,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\639\639.shp</t>
         </is>
       </c>
-      <c r="C7" s="16" t="n"/>
-      <c r="D7" s="16" t="n"/>
-      <c r="E7" s="16" t="n"/>
-      <c r="F7" s="15" t="inlineStr">
+      <c r="C7" s="15" t="n"/>
+      <c r="D7" s="15" t="n"/>
+      <c r="E7" s="15" t="n"/>
+      <c r="F7" s="14" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\6</t>
         </is>
       </c>
-      <c r="G7" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H7" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I7" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J7" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K7" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L7" s="17" t="inlineStr">
+      <c r="G7" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H7" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I7" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J7" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K7" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L7" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M7" s="14" t="inlineStr">
+      <c r="M7" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N7" s="16" t="n"/>
-      <c r="O7" s="7" t="n"/>
+      <c r="N7" s="15" t="n"/>
+      <c r="O7" s="6" t="n"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
-      <c r="A8" s="14" t="inlineStr">
+      <c r="A8" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -1042,54 +1036,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\640\640.shp</t>
         </is>
       </c>
-      <c r="C8" s="16" t="n"/>
-      <c r="D8" s="16" t="n"/>
-      <c r="E8" s="16" t="n"/>
-      <c r="F8" s="15" t="inlineStr">
+      <c r="C8" s="15" t="n"/>
+      <c r="D8" s="15" t="n"/>
+      <c r="E8" s="15" t="n"/>
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\7</t>
         </is>
       </c>
-      <c r="G8" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H8" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I8" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J8" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K8" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L8" s="17" t="inlineStr">
+      <c r="G8" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H8" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I8" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J8" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K8" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L8" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M8" s="14" t="inlineStr">
+      <c r="M8" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N8" s="16" t="n"/>
-      <c r="O8" s="7" t="n"/>
+      <c r="N8" s="15" t="n"/>
+      <c r="O8" s="6" t="n"/>
     </row>
     <row r="9" ht="19.5" customHeight="1">
-      <c r="A9" s="14" t="inlineStr">
+      <c r="A9" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -1099,54 +1093,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\641\641.shp</t>
         </is>
       </c>
-      <c r="C9" s="16" t="n"/>
-      <c r="D9" s="16" t="n"/>
-      <c r="E9" s="16" t="n"/>
-      <c r="F9" s="15" t="inlineStr">
+      <c r="C9" s="15" t="n"/>
+      <c r="D9" s="15" t="n"/>
+      <c r="E9" s="15" t="n"/>
+      <c r="F9" s="14" t="inlineStr">
         <is>
           <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\8</t>
         </is>
       </c>
-      <c r="G9" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H9" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I9" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J9" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K9" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L9" s="17" t="inlineStr">
+      <c r="G9" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H9" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I9" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J9" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K9" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L9" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M9" s="14" t="inlineStr">
+      <c r="M9" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N9" s="16" t="n"/>
-      <c r="O9" s="7" t="n"/>
+      <c r="N9" s="15" t="n"/>
+      <c r="O9" s="6" t="n"/>
     </row>
     <row r="10" ht="19.5" customHeight="1">
-      <c r="A10" s="14" t="inlineStr">
+      <c r="A10" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -1156,54 +1150,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\644\644.shp</t>
         </is>
       </c>
-      <c r="C10" s="16" t="n"/>
-      <c r="D10" s="16" t="n"/>
-      <c r="E10" s="16" t="n"/>
-      <c r="F10" s="15" t="inlineStr">
-        <is>
-          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS</t>
-        </is>
-      </c>
-      <c r="G10" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H10" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I10" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J10" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K10" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L10" s="17" t="inlineStr">
+      <c r="C10" s="15" t="n"/>
+      <c r="D10" s="15" t="n"/>
+      <c r="E10" s="15" t="n"/>
+      <c r="F10" s="14" t="inlineStr">
+        <is>
+          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\9</t>
+        </is>
+      </c>
+      <c r="G10" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H10" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I10" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J10" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K10" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L10" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M10" s="14" t="inlineStr">
+      <c r="M10" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N10" s="16" t="n"/>
-      <c r="O10" s="7" t="n"/>
+      <c r="N10" s="15" t="n"/>
+      <c r="O10" s="6" t="n"/>
     </row>
     <row r="11" ht="19.5" customHeight="1">
-      <c r="A11" s="14" t="inlineStr">
+      <c r="A11" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -1213,54 +1207,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\645\645.shp</t>
         </is>
       </c>
-      <c r="C11" s="16" t="n"/>
-      <c r="D11" s="16" t="n"/>
-      <c r="E11" s="16" t="n"/>
-      <c r="F11" s="15" t="inlineStr">
-        <is>
-          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS</t>
-        </is>
-      </c>
-      <c r="G11" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H11" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I11" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J11" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K11" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L11" s="17" t="inlineStr">
+      <c r="C11" s="15" t="n"/>
+      <c r="D11" s="15" t="n"/>
+      <c r="E11" s="15" t="n"/>
+      <c r="F11" s="14" t="inlineStr">
+        <is>
+          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\10</t>
+        </is>
+      </c>
+      <c r="G11" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H11" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I11" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J11" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K11" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L11" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M11" s="14" t="inlineStr">
+      <c r="M11" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N11" s="16" t="n"/>
-      <c r="O11" s="7" t="n"/>
+      <c r="N11" s="15" t="n"/>
+      <c r="O11" s="6" t="n"/>
     </row>
     <row r="12" ht="19.5" customHeight="1">
-      <c r="A12" s="14" t="inlineStr">
+      <c r="A12" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -1270,54 +1264,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\646\646.shp</t>
         </is>
       </c>
-      <c r="C12" s="16" t="n"/>
-      <c r="D12" s="16" t="n"/>
-      <c r="E12" s="16" t="n"/>
-      <c r="F12" s="15" t="inlineStr">
-        <is>
-          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS</t>
-        </is>
-      </c>
-      <c r="G12" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H12" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I12" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J12" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K12" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L12" s="17" t="inlineStr">
+      <c r="C12" s="15" t="n"/>
+      <c r="D12" s="15" t="n"/>
+      <c r="E12" s="15" t="n"/>
+      <c r="F12" s="14" t="inlineStr">
+        <is>
+          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\11</t>
+        </is>
+      </c>
+      <c r="G12" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H12" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I12" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J12" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K12" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L12" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M12" s="14" t="inlineStr">
+      <c r="M12" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N12" s="16" t="n"/>
-      <c r="O12" s="7" t="n"/>
+      <c r="N12" s="15" t="n"/>
+      <c r="O12" s="6" t="n"/>
     </row>
     <row r="13" ht="19.5" customHeight="1">
-      <c r="A13" s="14" t="inlineStr">
+      <c r="A13" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -1327,54 +1321,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\649\649.shp</t>
         </is>
       </c>
-      <c r="C13" s="16" t="n"/>
-      <c r="D13" s="16" t="n"/>
-      <c r="E13" s="16" t="n"/>
-      <c r="F13" s="15" t="inlineStr">
-        <is>
-          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS</t>
-        </is>
-      </c>
-      <c r="G13" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H13" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I13" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J13" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K13" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L13" s="17" t="inlineStr">
+      <c r="C13" s="15" t="n"/>
+      <c r="D13" s="15" t="n"/>
+      <c r="E13" s="15" t="n"/>
+      <c r="F13" s="14" t="inlineStr">
+        <is>
+          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\12</t>
+        </is>
+      </c>
+      <c r="G13" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H13" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I13" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J13" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K13" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L13" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M13" s="14" t="inlineStr">
+      <c r="M13" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N13" s="16" t="n"/>
-      <c r="O13" s="7" t="n"/>
+      <c r="N13" s="15" t="n"/>
+      <c r="O13" s="6" t="n"/>
     </row>
     <row r="14" ht="19.5" customHeight="1">
-      <c r="A14" s="14" t="inlineStr">
+      <c r="A14" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -1384,54 +1378,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\650\650.shp</t>
         </is>
       </c>
-      <c r="C14" s="16" t="n"/>
-      <c r="D14" s="16" t="n"/>
-      <c r="E14" s="16" t="n"/>
-      <c r="F14" s="15" t="inlineStr">
-        <is>
-          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS</t>
-        </is>
-      </c>
-      <c r="G14" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H14" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I14" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J14" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K14" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L14" s="17" t="inlineStr">
+      <c r="C14" s="15" t="n"/>
+      <c r="D14" s="15" t="n"/>
+      <c r="E14" s="15" t="n"/>
+      <c r="F14" s="14" t="inlineStr">
+        <is>
+          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\13</t>
+        </is>
+      </c>
+      <c r="G14" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H14" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I14" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J14" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K14" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L14" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M14" s="14" t="inlineStr">
+      <c r="M14" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N14" s="16" t="n"/>
-      <c r="O14" s="7" t="n"/>
+      <c r="N14" s="15" t="n"/>
+      <c r="O14" s="6" t="n"/>
     </row>
     <row r="15" ht="19.5" customHeight="1">
-      <c r="A15" s="14" t="inlineStr">
+      <c r="A15" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -1441,54 +1435,54 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\654\654.shp</t>
         </is>
       </c>
-      <c r="C15" s="16" t="n"/>
-      <c r="D15" s="16" t="n"/>
-      <c r="E15" s="16" t="n"/>
-      <c r="F15" s="15" t="inlineStr">
-        <is>
-          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS</t>
-        </is>
-      </c>
-      <c r="G15" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H15" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I15" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J15" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K15" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L15" s="17" t="inlineStr">
+      <c r="C15" s="15" t="n"/>
+      <c r="D15" s="15" t="n"/>
+      <c r="E15" s="15" t="n"/>
+      <c r="F15" s="14" t="inlineStr">
+        <is>
+          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\14</t>
+        </is>
+      </c>
+      <c r="G15" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H15" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I15" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J15" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K15" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L15" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M15" s="14" t="inlineStr">
+      <c r="M15" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N15" s="16" t="n"/>
-      <c r="O15" s="7" t="n"/>
+      <c r="N15" s="15" t="n"/>
+      <c r="O15" s="6" t="n"/>
     </row>
     <row r="16" ht="20.25" customHeight="1">
-      <c r="A16" s="14" t="inlineStr">
+      <c r="A16" s="13" t="inlineStr">
         <is>
           <t>South_Coast</t>
         </is>
@@ -1498,51 +1492,51 @@
           <t>\\spatialfiles.bcgov\srm\gss\projects\gr_2025_26_general_request_batch_20_statuses\source_data\Powell River Parcels - South Coast\655\655.shp</t>
         </is>
       </c>
-      <c r="C16" s="16" t="n"/>
-      <c r="D16" s="16" t="n"/>
-      <c r="E16" s="16" t="n"/>
-      <c r="F16" s="15" t="inlineStr">
-        <is>
-          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS</t>
-        </is>
-      </c>
-      <c r="G16" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H16" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I16" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J16" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K16" s="17" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L16" s="17" t="inlineStr">
+      <c r="C16" s="15" t="n"/>
+      <c r="D16" s="15" t="n"/>
+      <c r="E16" s="15" t="n"/>
+      <c r="F16" s="14" t="inlineStr">
+        <is>
+          <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\AST_OUTPUTS\15</t>
+        </is>
+      </c>
+      <c r="G16" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H16" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="I16" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J16" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K16" s="16" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L16" s="16" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="M16" s="14" t="inlineStr">
+      <c r="M16" s="17" t="inlineStr">
         <is>
           <t>Queued</t>
         </is>
       </c>
-      <c r="N16" s="16" t="n"/>
-      <c r="O16" s="7" t="n"/>
+      <c r="N16" s="15" t="n"/>
+      <c r="O16" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1566,9 +1560,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="27.14785714285714" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
+    <col width="27.14785714285714" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -1577,8 +1571,8 @@
           <t>Northeast</t>
         </is>
       </c>
-      <c r="B1" s="7" t="n"/>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="B1" s="6" t="n"/>
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>true</t>
         </is>
@@ -1590,8 +1584,8 @@
           <t>Cariboo</t>
         </is>
       </c>
-      <c r="B2" s="7" t="n"/>
-      <c r="C2" s="7" t="inlineStr">
+      <c r="B2" s="6" t="n"/>
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>false</t>
         </is>
@@ -1603,17 +1597,17 @@
           <t>Kootenay_Boundary</t>
         </is>
       </c>
-      <c r="B3" s="7" t="n"/>
-      <c r="C3" s="7" t="n"/>
+      <c r="B3" s="6" t="n"/>
+      <c r="C3" s="6" t="n"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Skeena</t>
         </is>
       </c>
-      <c r="B4" s="7" t="n"/>
-      <c r="C4" s="7" t="n"/>
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="6" t="n"/>
     </row>
     <row r="5" ht="18.75" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
@@ -1621,17 +1615,17 @@
           <t>South_Coast</t>
         </is>
       </c>
-      <c r="B5" s="7" t="n"/>
-      <c r="C5" s="7" t="n"/>
+      <c r="B5" s="6" t="n"/>
+      <c r="C5" s="6" t="n"/>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Thompson_Okanagan</t>
         </is>
       </c>
-      <c r="B6" s="7" t="n"/>
-      <c r="C6" s="7" t="n"/>
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="6" t="n"/>
     </row>
     <row r="7" ht="18.75" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
@@ -1639,17 +1633,17 @@
           <t>West_Coast</t>
         </is>
       </c>
-      <c r="B7" s="7" t="n"/>
-      <c r="C7" s="7" t="n"/>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="6" t="n"/>
     </row>
     <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" s="5" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Omineca</t>
         </is>
       </c>
-      <c r="B8" s="7" t="n"/>
-      <c r="C8" s="7" t="n"/>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="6" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cleaned up Excel File. V3 BCGW Connection is working
</commit_message>
<xml_diff>
--- a/autoast/auto_ast_v3_Breville_folium_maps/gr_2025_26_jobs.xlsx
+++ b/autoast/auto_ast_v3_Breville_folium_maps/gr_2025_26_jobs.xlsx
@@ -591,7 +591,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="23.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="145.7192857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
@@ -734,7 +734,7 @@
       </c>
       <c r="M2" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N2" s="18" t="n"/>
@@ -791,7 +791,7 @@
       </c>
       <c r="M3" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N3" s="18" t="n"/>
@@ -848,7 +848,7 @@
       </c>
       <c r="M4" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N4" s="15" t="n"/>
@@ -905,7 +905,7 @@
       </c>
       <c r="M5" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N5" s="15" t="n"/>
@@ -962,7 +962,7 @@
       </c>
       <c r="M6" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N6" s="15" t="n"/>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="M7" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N7" s="15" t="n"/>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="M8" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N8" s="15" t="n"/>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="M9" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N9" s="15" t="n"/>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="M10" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N10" s="15" t="n"/>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="M11" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N11" s="15" t="n"/>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="M12" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N12" s="15" t="n"/>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="M13" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N13" s="15" t="n"/>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="M14" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N14" s="15" t="n"/>
@@ -1475,7 +1475,7 @@
       </c>
       <c r="M15" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N15" s="15" t="n"/>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="M16" s="17" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>COMPLETE</t>
         </is>
       </c>
       <c r="N16" s="15" t="n"/>
@@ -1558,7 +1558,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="27.14785714285714" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>

</xml_diff>